<commit_message>
Project pr2 is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/pr2/Main.xlsx
+++ b/DESIGN/rules/pr2/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1046,8 +1047,8 @@
       <c r="C8" s="16">
         <v>0</v>
       </c>
-      <c r="D8" s="17">
-        <v>11</v>
+      <c r="D8" s="17" t="n">
+        <v>112.0</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Restored from revision of DEFAULT on 12/20/2021 03:54:35 PM. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/pr2/Main.xlsx
+++ b/DESIGN/rules/pr2/Main.xlsx
@@ -966,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1044,8 +1044,8 @@
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16">
-        <v>0</v>
+      <c r="C8" s="16" t="n">
+        <v>11.0</v>
       </c>
       <c r="D8" s="17" t="n">
         <v>112.0</v>

</xml_diff>